<commit_message>
adding resources, and updates to labs
</commit_message>
<xml_diff>
--- a/CS320-Sp24-Draft-Schedule.xlsx
+++ b/CS320-Sp24-Draft-Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E8B397-8605-4F4B-B0A6-C2682C3009A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2A6AE8-DEF6-4737-8D5A-D8BA6A370202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="0" windowWidth="26850" windowHeight="15428" xr2:uid="{28923DA2-90DB-47E2-B94E-ECFE9B6BB1C0}"/>
+    <workbookView xWindow="1643" yWindow="68" windowWidth="27075" windowHeight="15427" xr2:uid="{28923DA2-90DB-47E2-B94E-ECFE9B6BB1C0}"/>
   </bookViews>
   <sheets>
     <sheet name="CS320-Prelim Scheudle" sheetId="1" r:id="rId1"/>
@@ -872,7 +872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AB1940-B34F-4F83-BCB8-E449ECD30E0E}">
   <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>